<commit_message>
added getCellData for int value. Everything works
</commit_message>
<xml_diff>
--- a/src/test/excel/Book2.xlsx
+++ b/src/test/excel/Book2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24800" windowHeight="9440"/>
+    <workbookView windowWidth="24800" windowHeight="9220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
   <si>
     <t>gameData</t>
   </si>
@@ -31,27 +31,18 @@
     <t>Input is incorrect</t>
   </si>
   <si>
-    <t>"500"</t>
-  </si>
-  <si>
     <t>xxxooo---</t>
   </si>
   <si>
     <t>Status is incorrect</t>
   </si>
   <si>
-    <t>"404"</t>
-  </si>
-  <si>
     <t>x--------</t>
   </si>
   <si>
     <t>Game continues</t>
   </si>
   <si>
-    <t>"100"</t>
-  </si>
-  <si>
     <t>xxoo-----</t>
   </si>
   <si>
@@ -61,16 +52,10 @@
     <t>x won</t>
   </si>
   <si>
-    <t>"301"</t>
-  </si>
-  <si>
     <t>xxoxx-ooo</t>
   </si>
   <si>
     <t>o won</t>
-  </si>
-  <si>
-    <t>"302"</t>
   </si>
 </sst>
 </file>
@@ -78,9 +63,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -113,6 +98,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -128,10 +159,49 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -143,36 +213,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -180,15 +220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -196,55 +227,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -265,49 +250,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,127 +412,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,6 +435,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -488,24 +512,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -521,32 +527,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -555,139 +540,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -696,7 +681,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1035,7 +1020,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1063,63 +1048,63 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="C2" s="3">
+        <v>500</v>
       </c>
     </row>
     <row r="3" ht="15" spans="1:3">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
+      <c r="C3" s="3">
+        <v>404</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="3">
+        <v>301</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>